<commit_message>
fixes #186, add media_types relation, fix bugs
</commit_message>
<xml_diff>
--- a/spec/fixtures/io_files/Collective_IO_video_li.xlsx
+++ b/spec/fixtures/io_files/Collective_IO_video_li.xlsx
@@ -23,21 +23,24 @@
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0" vbProcedure="false">'Standard Specs'!$A$1:$Q$11</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Standard Specs'!$A$1:$Q$11</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Standard Specs'!$A$1:$Q$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Standard Specs'!$A$1:$Q$11</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">'Rich Media Specs'!$A$1:$Z$11</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area_0" vbProcedure="false">'Rich Media Specs'!$A$1:$Z$11</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Rich Media Specs'!$A$1:$Z$11</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Rich Media Specs'!$A$1:$Z$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Rich Media Specs'!$A$1:$Z$11</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area" vbProcedure="false">'Video Specs'!$A$1:$O$8</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area_0" vbProcedure="false">'Video Specs'!$A$1:$O$8</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Video Specs'!$A$1:$O$8</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Video Specs'!$A$1:$O$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Video Specs'!$A$1:$O$8</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="175">
   <si>
     <t>Date:</t>
   </si>
@@ -179,10 +182,13 @@
     <t>Media Cost (Net)</t>
   </si>
   <si>
+    <t>Video Pre-Roll and 300X250 Companion Ad</t>
+  </si>
+  <si>
+    <t>Age 18-34 or Age 34-50 or Education; Columbus Zips</t>
+  </si>
+  <si>
     <t>Pre-Roll and 300X250 Companion Ad</t>
-  </si>
-  <si>
-    <t>Age 18-34 or Age 34-50 or Education; Columbus Zips</t>
   </si>
   <si>
     <t>RON; Columbus Zips</t>
@@ -1395,7 +1401,7 @@
     <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
     <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
     <cellStyle builtinId="8" customBuiltin="false" name="*unknown*" xfId="20"/>
-    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Excel Built-in Excel Built-in Normal 2" xfId="21"/>
+    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal 2" xfId="21"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1465,15 +1471,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>212760</xdr:colOff>
+      <xdr:colOff>239760</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>50040</xdr:rowOff>
+      <xdr:rowOff>41040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>445320</xdr:colOff>
+      <xdr:colOff>471960</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>95760</xdr:rowOff>
+      <xdr:rowOff>86400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1488,8 +1494,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="212760" y="192600"/>
-          <a:ext cx="1230480" cy="598320"/>
+          <a:off x="239760" y="183600"/>
+          <a:ext cx="1230120" cy="597960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1504,15 +1510,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>108000</xdr:colOff>
+      <xdr:colOff>135000</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>30600</xdr:rowOff>
+      <xdr:rowOff>21600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>1335600</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>11520</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>29160</xdr:rowOff>
+      <xdr:rowOff>19800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1521,8 +1527,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="108000" y="30600"/>
-          <a:ext cx="12354480" cy="46080"/>
+          <a:off x="135000" y="21600"/>
+          <a:ext cx="12354120" cy="45720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1543,15 +1549,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>108000</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>2160</xdr:rowOff>
+      <xdr:colOff>135000</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>155160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>1335600</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>11520</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>47520</xdr:rowOff>
+      <xdr:rowOff>38160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1560,8 +1566,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="108000" y="859320"/>
-          <a:ext cx="12354480" cy="45360"/>
+          <a:off x="135000" y="850320"/>
+          <a:ext cx="12354120" cy="45000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1582,15 +1588,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>108000</xdr:colOff>
+      <xdr:colOff>135000</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>151560</xdr:rowOff>
+      <xdr:rowOff>142560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>22680</xdr:colOff>
+      <xdr:colOff>49320</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>131400</xdr:rowOff>
+      <xdr:rowOff>122040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1599,8 +1605,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="108000" y="4734000"/>
-          <a:ext cx="12392280" cy="141840"/>
+          <a:off x="135000" y="4725000"/>
+          <a:ext cx="12391920" cy="141480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1621,15 +1627,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>108000</xdr:colOff>
+      <xdr:colOff>135000</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>132120</xdr:rowOff>
+      <xdr:rowOff>123120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>13320</xdr:colOff>
+      <xdr:colOff>39960</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>15120</xdr:rowOff>
+      <xdr:rowOff>5760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1638,8 +1644,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="108000" y="2945160"/>
-          <a:ext cx="12382920" cy="44640"/>
+          <a:off x="135000" y="2936160"/>
+          <a:ext cx="12382560" cy="44280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1665,15 +1671,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>165240</xdr:colOff>
+      <xdr:colOff>192240</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>21240</xdr:rowOff>
+      <xdr:rowOff>12240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>230400</xdr:colOff>
+      <xdr:colOff>257040</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>219960</xdr:rowOff>
+      <xdr:rowOff>210600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1688,8 +1694,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="165240" y="21240"/>
-          <a:ext cx="1596600" cy="722520"/>
+          <a:off x="192240" y="12240"/>
+          <a:ext cx="1596240" cy="722160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1709,15 +1715,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>212760</xdr:colOff>
+      <xdr:colOff>239760</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>78480</xdr:rowOff>
+      <xdr:rowOff>69480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>277920</xdr:colOff>
+      <xdr:colOff>304560</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>277200</xdr:rowOff>
+      <xdr:rowOff>267840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1732,8 +1738,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="212760" y="78480"/>
-          <a:ext cx="1596600" cy="722520"/>
+          <a:off x="239760" y="69480"/>
+          <a:ext cx="1596240" cy="722160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1753,15 +1759,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>212760</xdr:colOff>
+      <xdr:colOff>239760</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>30600</xdr:rowOff>
+      <xdr:rowOff>21600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>277920</xdr:colOff>
+      <xdr:colOff>304560</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>229320</xdr:rowOff>
+      <xdr:rowOff>219960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1776,8 +1782,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="212760" y="30600"/>
-          <a:ext cx="1596600" cy="722520"/>
+          <a:off x="239760" y="21600"/>
+          <a:ext cx="1596240" cy="722160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1797,13 +1803,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:AI65536"/>
+  <dimension ref="A1:AI172"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="false" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A16" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="F30" activeCellId="0" pane="topLeft" sqref="F30"/>
+      <selection activeCell="C30" activeCellId="0" pane="topLeft" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.1479591836735"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.4183673469388"/>
@@ -2609,10 +2615,10 @@
         <v>41515</v>
       </c>
       <c r="C30" s="56" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D30" s="61" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E30" s="61"/>
       <c r="F30" s="58" t="n">
@@ -2624,7 +2630,7 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="31" s="5">
       <c r="A31" s="62" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B31" s="62"/>
       <c r="C31" s="62"/>
@@ -2684,10 +2690,10 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="21.75" outlineLevel="0" r="33" s="5">
       <c r="A33" s="68" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B33" s="69" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C33" s="69"/>
       <c r="D33" s="69"/>
@@ -2780,7 +2786,7 @@
       <c r="G36" s="4"/>
       <c r="H36" s="44"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="37" s="5">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="37">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
@@ -2790,13 +2796,13 @@
       <c r="G37" s="4"/>
       <c r="H37" s="4"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="38" s="5">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="38">
       <c r="A38" s="70" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B38" s="71"/>
       <c r="C38" s="72" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D38" s="71"/>
       <c r="E38" s="71"/>
@@ -2804,11 +2810,11 @@
       <c r="G38" s="71"/>
       <c r="H38" s="71"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="39" s="5">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="39">
       <c r="A39" s="70"/>
       <c r="B39" s="71"/>
       <c r="C39" s="72" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D39" s="71"/>
       <c r="E39" s="71"/>
@@ -2816,7 +2822,7 @@
       <c r="G39" s="71"/>
       <c r="H39" s="71"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="40" s="5">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="40">
       <c r="A40" s="71"/>
       <c r="B40" s="71"/>
       <c r="C40" s="71"/>
@@ -2826,13 +2832,13 @@
       <c r="G40" s="71"/>
       <c r="H40" s="71"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="41" s="5">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="41">
       <c r="A41" s="72" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B41" s="71"/>
       <c r="C41" s="72" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D41" s="71"/>
       <c r="E41" s="71"/>
@@ -2840,7 +2846,7 @@
       <c r="G41" s="71"/>
       <c r="H41" s="71"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="42" s="5">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="42">
       <c r="A42" s="71"/>
       <c r="B42" s="71"/>
       <c r="C42" s="71"/>
@@ -2850,13 +2856,13 @@
       <c r="G42" s="71"/>
       <c r="H42" s="71"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="43" s="5">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="43">
       <c r="A43" s="72" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B43" s="71"/>
       <c r="C43" s="73" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D43" s="73"/>
       <c r="E43" s="73"/>
@@ -2864,7 +2870,7 @@
       <c r="G43" s="73"/>
       <c r="H43" s="73"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="44" s="5">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="44">
       <c r="A44" s="71"/>
       <c r="B44" s="71"/>
       <c r="C44" s="73"/>
@@ -2874,7 +2880,7 @@
       <c r="G44" s="73"/>
       <c r="H44" s="73"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="45" s="5">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="45">
       <c r="A45" s="71"/>
       <c r="B45" s="71"/>
       <c r="C45" s="74"/>
@@ -2884,13 +2890,13 @@
       <c r="G45" s="74"/>
       <c r="H45" s="74"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="46" s="5">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="46">
       <c r="A46" s="72" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B46" s="72"/>
       <c r="C46" s="75" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D46" s="75"/>
       <c r="E46" s="75"/>
@@ -2898,7 +2904,7 @@
       <c r="G46" s="75"/>
       <c r="H46" s="75"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="47" s="5">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="47">
       <c r="A47" s="72"/>
       <c r="B47" s="72"/>
       <c r="C47" s="75"/>
@@ -2908,7 +2914,7 @@
       <c r="G47" s="75"/>
       <c r="H47" s="75"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="48" s="5">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="48">
       <c r="A48" s="72"/>
       <c r="B48" s="72"/>
       <c r="C48" s="75"/>
@@ -2918,7 +2924,7 @@
       <c r="G48" s="75"/>
       <c r="H48" s="75"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="49" s="5">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="49">
       <c r="A49" s="72"/>
       <c r="B49" s="72"/>
       <c r="C49" s="76"/>
@@ -2928,13 +2934,13 @@
       <c r="G49" s="76"/>
       <c r="H49" s="76"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="50" s="5">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="50">
       <c r="A50" s="72" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B50" s="72"/>
       <c r="C50" s="75" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D50" s="75"/>
       <c r="E50" s="75"/>
@@ -2942,7 +2948,7 @@
       <c r="G50" s="75"/>
       <c r="H50" s="75"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="51" s="5">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="51">
       <c r="A51" s="72"/>
       <c r="B51" s="72"/>
       <c r="C51" s="75"/>
@@ -2952,7 +2958,7 @@
       <c r="G51" s="75"/>
       <c r="H51" s="75"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="52" s="5">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="52">
       <c r="A52" s="72"/>
       <c r="B52" s="72"/>
       <c r="C52" s="75"/>
@@ -2962,7 +2968,7 @@
       <c r="G52" s="75"/>
       <c r="H52" s="75"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="53" s="5">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="53">
       <c r="A53" s="72"/>
       <c r="B53" s="72"/>
       <c r="C53" s="76"/>
@@ -2974,11 +2980,11 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="54">
       <c r="A54" s="72" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B54" s="72"/>
       <c r="C54" s="75" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D54" s="75"/>
       <c r="E54" s="75"/>
@@ -3018,7 +3024,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="58">
       <c r="A58" s="72" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B58" s="72"/>
       <c r="C58" s="72"/>
@@ -3070,17 +3076,17 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="63">
       <c r="A63" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
       <c r="D63" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E63" s="4"/>
       <c r="F63" s="4"/>
       <c r="G63" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H63" s="4"/>
     </row>
@@ -4118,7 +4124,7 @@
       <c r="G134" s="4"/>
       <c r="H134" s="4"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="135" s="5">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="135">
       <c r="A135" s="4"/>
       <c r="B135" s="4"/>
       <c r="C135" s="4"/>
@@ -4129,7 +4135,7 @@
       <c r="H135" s="4"/>
       <c r="I135" s="28"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="136" s="5">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="136">
       <c r="A136" s="4"/>
       <c r="B136" s="4"/>
       <c r="C136" s="4"/>
@@ -4140,7 +4146,7 @@
       <c r="H136" s="4"/>
       <c r="I136" s="28"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="137" s="5">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="137">
       <c r="A137" s="4"/>
       <c r="B137" s="4"/>
       <c r="C137" s="4"/>
@@ -4151,7 +4157,7 @@
       <c r="H137" s="4"/>
       <c r="I137" s="28"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="138" s="5">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="138">
       <c r="A138" s="4"/>
       <c r="B138" s="4"/>
       <c r="C138" s="4"/>
@@ -4162,7 +4168,7 @@
       <c r="H138" s="4"/>
       <c r="I138" s="28"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="139" s="5">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="139">
       <c r="A139" s="4"/>
       <c r="B139" s="4"/>
       <c r="C139" s="4"/>
@@ -4173,7 +4179,7 @@
       <c r="H139" s="4"/>
       <c r="I139" s="28"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="8.1" outlineLevel="0" r="140" s="5">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="8.1" outlineLevel="0" r="140">
       <c r="A140" s="4"/>
       <c r="B140" s="4"/>
       <c r="C140" s="4"/>
@@ -4184,7 +4190,7 @@
       <c r="H140" s="4"/>
       <c r="I140" s="28"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="81" outlineLevel="0" r="141" s="5">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="81" outlineLevel="0" r="141">
       <c r="A141" s="4"/>
       <c r="B141" s="4"/>
       <c r="C141" s="4"/>
@@ -4272,18 +4278,9 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="172">
       <c r="I172" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048568"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048569"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048570"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048571"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048572"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048573"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048574"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048575"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048576"/>
+        <v>65</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="21">
     <mergeCell ref="D5:G6"/>
@@ -4352,25 +4349,25 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="3">
       <c r="A3" s="78" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B3" s="78"/>
       <c r="C3" s="78"/>
       <c r="D3" s="78"/>
       <c r="E3" s="78" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F3" s="78"/>
       <c r="G3" s="78" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H3" s="78" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I3" s="78" t="s">
         <v>36</v>
@@ -4379,13 +4376,13 @@
         <v>37</v>
       </c>
       <c r="K3" s="78" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="L3" s="78" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="P3" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="4">
@@ -4394,26 +4391,26 @@
         <v>0</v>
       </c>
       <c r="B4" s="80" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C4" s="80" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D4" s="80" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E4" s="81" t="n">
         <v>78002775</v>
       </c>
       <c r="F4" s="79" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G4" s="79" t="str">
         <f aca="false">'Insertion Order'!D29</f>
         <v>Age 18-34 or Age 34-50 or Education; Columbus Zips</v>
       </c>
       <c r="H4" s="79" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I4" s="82" t="n">
         <f aca="false">'Insertion Order'!H25</f>
@@ -4432,7 +4429,7 @@
         <v>http://ad.doubleclick.net/jump/.collective;adid=78002775;sz=300x250</v>
       </c>
       <c r="P4" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="5">
@@ -4441,24 +4438,24 @@
         <v>0</v>
       </c>
       <c r="B5" s="80" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C5" s="80" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D5" s="80" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E5" s="79"/>
       <c r="F5" s="79" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G5" s="79" t="str">
         <f aca="false">'Insertion Order'!D30</f>
         <v>RON; Columbus Zips</v>
       </c>
       <c r="H5" s="79" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I5" s="82" t="n">
         <f aca="false">'Insertion Order'!H25</f>
@@ -4483,24 +4480,24 @@
         <v>0</v>
       </c>
       <c r="B6" s="80" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C6" s="80" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D6" s="80" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E6" s="79"/>
       <c r="F6" s="79" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G6" s="79" t="str">
         <f aca="false">'Insertion Order'!D30</f>
         <v>RON; Columbus Zips</v>
       </c>
       <c r="H6" s="79" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I6" s="82" t="n">
         <f aca="false">'Insertion Order'!H25</f>
@@ -4519,7 +4516,7 @@
         <v>http://ad.doubleclick.net/jump/.collective;adid=;sz=160x600</v>
       </c>
       <c r="P6" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="7">
@@ -4528,24 +4525,24 @@
         <v>0</v>
       </c>
       <c r="B7" s="80" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C7" s="80" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D7" s="80" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E7" s="79"/>
       <c r="F7" s="79" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G7" s="79" t="str">
         <f aca="false">'Insertion Order'!$D$30</f>
         <v>RON; Columbus Zips</v>
       </c>
       <c r="H7" s="79" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I7" s="82" t="n">
         <f aca="false">'Insertion Order'!H25</f>
@@ -4564,7 +4561,7 @@
         <v>http://ad.doubleclick.net/jump/.collective;adid=;sz=300x250</v>
       </c>
       <c r="P7" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="8">
@@ -4573,24 +4570,24 @@
         <v>0</v>
       </c>
       <c r="B8" s="80" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C8" s="80" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D8" s="80" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E8" s="83"/>
       <c r="F8" s="79" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G8" s="79" t="str">
         <f aca="false">'Insertion Order'!$D$30</f>
         <v>RON; Columbus Zips</v>
       </c>
       <c r="H8" s="79" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I8" s="82" t="n">
         <f aca="false">'Insertion Order'!H25</f>
@@ -4609,7 +4606,7 @@
         <v>http://ad.doubleclick.net/jump/.collective;adid=;sz=728x90</v>
       </c>
       <c r="P8" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="9">
@@ -4618,24 +4615,24 @@
         <v>0</v>
       </c>
       <c r="B9" s="80" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C9" s="80" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D9" s="80" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E9" s="79"/>
       <c r="F9" s="79" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G9" s="79" t="str">
         <f aca="false">'Insertion Order'!$D$30</f>
         <v>RON; Columbus Zips</v>
       </c>
       <c r="H9" s="79" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I9" s="82" t="n">
         <f aca="false">'Insertion Order'!H25</f>
@@ -4656,22 +4653,22 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="10">
       <c r="R10" s="78" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="11">
       <c r="R11" s="79" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="12">
       <c r="R12" s="79" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="13">
       <c r="R13" s="79" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -4730,7 +4727,7 @@
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="3">
       <c r="C3" s="84"/>
       <c r="D3" s="85" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E3" s="86"/>
       <c r="F3" s="86"/>
@@ -4739,55 +4736,55 @@
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="26.1" outlineLevel="0" r="4"/>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="39" outlineLevel="0" r="5" s="90">
       <c r="A5" s="87" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B5" s="87" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C5" s="87" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D5" s="87" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E5" s="87" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F5" s="87" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G5" s="87" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H5" s="88" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I5" s="87" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J5" s="87" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="K5" s="87" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L5" s="87" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="M5" s="88" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="N5" s="88" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="O5" s="88" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="P5" s="88" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="Q5" s="87" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="R5" s="89"/>
     </row>
@@ -4813,260 +4810,260 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="7" s="101">
       <c r="A7" s="94" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B7" s="94" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C7" s="95" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D7" s="94" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E7" s="94" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F7" s="94" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G7" s="95" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H7" s="96" t="n">
         <v>8</v>
       </c>
       <c r="I7" s="95" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="J7" s="95" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="K7" s="94" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="L7" s="94" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="M7" s="96" t="n">
         <v>20</v>
       </c>
       <c r="N7" s="97" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="O7" s="96" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="P7" s="98" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="Q7" s="99"/>
       <c r="R7" s="100"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="8" s="101">
       <c r="A8" s="94" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B8" s="94" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C8" s="95" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D8" s="94" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E8" s="94" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F8" s="94" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G8" s="95" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H8" s="96" t="n">
         <v>8</v>
       </c>
       <c r="I8" s="95" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="J8" s="95" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="K8" s="94" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="L8" s="94" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="M8" s="96" t="n">
         <v>20</v>
       </c>
       <c r="N8" s="97" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="O8" s="96" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="P8" s="98" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="Q8" s="99"/>
       <c r="R8" s="100"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="9" s="101">
       <c r="A9" s="94" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B9" s="94" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C9" s="95" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D9" s="94" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E9" s="94" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F9" s="94" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G9" s="95" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H9" s="96" t="n">
         <v>8</v>
       </c>
       <c r="I9" s="95" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="J9" s="95" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="K9" s="94" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="L9" s="94" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="M9" s="96" t="n">
         <v>20</v>
       </c>
       <c r="N9" s="97" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="O9" s="96" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="P9" s="98" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="Q9" s="99"/>
       <c r="R9" s="100"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="10" s="101">
       <c r="A10" s="94" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B10" s="94" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C10" s="95" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D10" s="94" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E10" s="94" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F10" s="94" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G10" s="95" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H10" s="96" t="n">
         <v>8</v>
       </c>
       <c r="I10" s="95" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="J10" s="95" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="K10" s="94" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="L10" s="94" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="M10" s="96" t="n">
         <v>20</v>
       </c>
       <c r="N10" s="97" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="O10" s="96" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="P10" s="98" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="Q10" s="99"/>
       <c r="R10" s="100"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="64.5" outlineLevel="0" r="11" s="101">
       <c r="A11" s="94" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B11" s="94" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C11" s="95" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D11" s="94" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E11" s="94" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F11" s="94" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G11" s="95" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H11" s="96" t="n">
         <v>8</v>
       </c>
       <c r="I11" s="95" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="J11" s="95" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="K11" s="94" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="L11" s="94" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="M11" s="96" t="n">
         <v>20</v>
       </c>
       <c r="N11" s="97" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="O11" s="96" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="P11" s="98" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="Q11" s="99"/>
       <c r="R11" s="100"/>
@@ -5143,88 +5140,88 @@
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="3">
       <c r="C3" s="84"/>
       <c r="D3" s="85" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="36" outlineLevel="0" r="4"/>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="51.75" outlineLevel="0" r="5" s="90">
       <c r="A5" s="87" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B5" s="87" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C5" s="87" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D5" s="87" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E5" s="87" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F5" s="87" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G5" s="87" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H5" s="87" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="I5" s="87" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="J5" s="88" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="K5" s="87" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="L5" s="87" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="M5" s="87" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="N5" s="88" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="O5" s="88" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="P5" s="88" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="Q5" s="88" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="R5" s="88" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="S5" s="88" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="T5" s="88" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="U5" s="88" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="V5" s="87" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="W5" s="88" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="X5" s="88" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="Y5" s="88" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="Z5" s="87" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="AA5" s="89"/>
     </row>
@@ -5259,395 +5256,395 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="7" s="101">
       <c r="A7" s="94" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B7" s="94" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C7" s="95" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D7" s="94" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E7" s="94" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F7" s="94" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G7" s="94" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H7" s="94" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="I7" s="95" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="J7" s="96" t="n">
         <v>8</v>
       </c>
       <c r="K7" s="95" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="L7" s="94" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="M7" s="94" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="N7" s="96" t="n">
         <v>24</v>
       </c>
       <c r="O7" s="97" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="P7" s="96" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="Q7" s="97" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="R7" s="97" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="S7" s="105" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="T7" s="96" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="U7" s="96" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="V7" s="95" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="W7" s="97" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="X7" s="96" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="Y7" s="106" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="Z7" s="99"/>
       <c r="AA7" s="100"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="8" s="101">
       <c r="A8" s="94" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B8" s="94" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C8" s="95" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D8" s="94" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E8" s="94" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F8" s="94" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G8" s="94" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H8" s="94" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="I8" s="95" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="J8" s="96" t="n">
         <v>8</v>
       </c>
       <c r="K8" s="95" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="L8" s="94" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="M8" s="94" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="N8" s="96" t="n">
         <v>24</v>
       </c>
       <c r="O8" s="97" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="P8" s="96" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="Q8" s="97" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="R8" s="97" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="S8" s="105" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="T8" s="96" t="s">
+        <v>146</v>
+      </c>
+      <c r="U8" s="96" t="s">
+        <v>147</v>
+      </c>
+      <c r="V8" s="95" t="s">
+        <v>144</v>
+      </c>
+      <c r="W8" s="97" t="s">
         <v>145</v>
       </c>
-      <c r="U8" s="96" t="s">
-        <v>146</v>
-      </c>
-      <c r="V8" s="95" t="s">
-        <v>143</v>
-      </c>
-      <c r="W8" s="97" t="s">
-        <v>144</v>
-      </c>
       <c r="X8" s="96" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="Y8" s="106" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="Z8" s="99"/>
       <c r="AA8" s="100"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="9" s="101">
       <c r="A9" s="94" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B9" s="94" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C9" s="95" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D9" s="94" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E9" s="94" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F9" s="94" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G9" s="94" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H9" s="94" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="I9" s="95" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="J9" s="96" t="n">
         <v>8</v>
       </c>
       <c r="K9" s="95" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="L9" s="94" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="M9" s="94" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="N9" s="96" t="n">
         <v>24</v>
       </c>
       <c r="O9" s="97" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="P9" s="96" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="Q9" s="97" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="R9" s="97" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="S9" s="105" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="T9" s="96" t="s">
+        <v>148</v>
+      </c>
+      <c r="U9" s="96" t="s">
         <v>147</v>
       </c>
-      <c r="U9" s="96" t="s">
-        <v>146</v>
-      </c>
       <c r="V9" s="95" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="W9" s="97" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="X9" s="96" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="Y9" s="106" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="Z9" s="99"/>
       <c r="AA9" s="100"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="10" s="101">
       <c r="A10" s="94" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B10" s="94" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C10" s="95" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D10" s="94" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E10" s="94" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F10" s="94" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G10" s="94" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H10" s="94" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="I10" s="95" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="J10" s="96" t="n">
         <v>8</v>
       </c>
       <c r="K10" s="95" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="L10" s="94" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="M10" s="94" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="N10" s="96" t="n">
         <v>24</v>
       </c>
       <c r="O10" s="97" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="P10" s="96" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="Q10" s="97" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="R10" s="97" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="S10" s="105" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="T10" s="96" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="U10" s="96" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="V10" s="95" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="W10" s="97" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="X10" s="96" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="Y10" s="106" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="Z10" s="99"/>
       <c r="AA10" s="100"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="64.5" outlineLevel="0" r="11">
       <c r="A11" s="94" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B11" s="94" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C11" s="95" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D11" s="94" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E11" s="94" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F11" s="94" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G11" s="94" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H11" s="94" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="I11" s="95" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="J11" s="96" t="n">
         <v>8</v>
       </c>
       <c r="K11" s="95" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="L11" s="94" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="M11" s="94" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="N11" s="107" t="n">
         <v>24</v>
       </c>
       <c r="O11" s="108" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="P11" s="96" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="Q11" s="97" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="R11" s="97" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="S11" s="105" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="T11" s="96" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="U11" s="96" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="V11" s="95" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="W11" s="97" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="X11" s="96" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="Y11" s="106" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="Z11" s="99"/>
       <c r="AA11" s="100"/>
@@ -5725,7 +5722,7 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="3">
       <c r="C3" s="109" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D3" s="85"/>
       <c r="E3" s="85"/>
@@ -5735,49 +5732,49 @@
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="33.95" outlineLevel="0" r="4"/>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="39" outlineLevel="0" r="5" s="90">
       <c r="A5" s="87" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B5" s="111" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C5" s="87" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D5" s="87" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E5" s="87" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F5" s="87" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="G5" s="87" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H5" s="87" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="I5" s="87" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="J5" s="88" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="K5" s="88" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="L5" s="88" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="M5" s="88" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="N5" s="88" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="O5" s="87" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="P5" s="89"/>
     </row>
@@ -5801,97 +5798,97 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="7" s="101">
       <c r="A7" s="94" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B7" s="112" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C7" s="95" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D7" s="94" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E7" s="94" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="F7" s="94" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="G7" s="94" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H7" s="94" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="I7" s="94" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="J7" s="96" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="K7" s="96" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="L7" s="97" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="M7" s="96" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="N7" s="106" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="O7" s="113" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="P7" s="100"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="64.5" outlineLevel="0" r="8">
       <c r="A8" s="94" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B8" s="112" t="s">
+        <v>172</v>
+      </c>
+      <c r="C8" s="95" t="s">
+        <v>173</v>
+      </c>
+      <c r="D8" s="94" t="s">
+        <v>174</v>
+      </c>
+      <c r="E8" s="114" t="s">
+        <v>163</v>
+      </c>
+      <c r="F8" s="94" t="s">
+        <v>164</v>
+      </c>
+      <c r="G8" s="114" t="s">
+        <v>165</v>
+      </c>
+      <c r="H8" s="114" t="s">
+        <v>166</v>
+      </c>
+      <c r="I8" s="94" t="s">
+        <v>167</v>
+      </c>
+      <c r="J8" s="96" t="s">
+        <v>168</v>
+      </c>
+      <c r="K8" s="96" t="s">
+        <v>79</v>
+      </c>
+      <c r="L8" s="97" t="s">
+        <v>169</v>
+      </c>
+      <c r="M8" s="96" t="s">
+        <v>170</v>
+      </c>
+      <c r="N8" s="106" t="s">
+        <v>115</v>
+      </c>
+      <c r="O8" s="113" t="s">
         <v>171</v>
-      </c>
-      <c r="C8" s="95" t="s">
-        <v>172</v>
-      </c>
-      <c r="D8" s="94" t="s">
-        <v>173</v>
-      </c>
-      <c r="E8" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="F8" s="94" t="s">
-        <v>163</v>
-      </c>
-      <c r="G8" s="114" t="s">
-        <v>164</v>
-      </c>
-      <c r="H8" s="114" t="s">
-        <v>165</v>
-      </c>
-      <c r="I8" s="94" t="s">
-        <v>166</v>
-      </c>
-      <c r="J8" s="96" t="s">
-        <v>167</v>
-      </c>
-      <c r="K8" s="96" t="s">
-        <v>78</v>
-      </c>
-      <c r="L8" s="97" t="s">
-        <v>168</v>
-      </c>
-      <c r="M8" s="96" t="s">
-        <v>169</v>
-      </c>
-      <c r="N8" s="106" t="s">
-        <v>114</v>
-      </c>
-      <c r="O8" s="113" t="s">
-        <v>170</v>
       </c>
       <c r="P8" s="100"/>
     </row>

</xml_diff>

<commit_message>
fix #186, add 1x1 pattern matching
</commit_message>
<xml_diff>
--- a/spec/fixtures/io_files/Collective_IO_video_li.xlsx
+++ b/spec/fixtures/io_files/Collective_IO_video_li.xlsx
@@ -24,16 +24,19 @@
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Standard Specs'!$A$1:$Q$11</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Standard Specs'!$A$1:$Q$11</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Standard Specs'!$A$1:$Q$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Standard Specs'!$A$1:$Q$11</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">'Rich Media Specs'!$A$1:$Z$11</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area_0" vbProcedure="false">'Rich Media Specs'!$A$1:$Z$11</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Rich Media Specs'!$A$1:$Z$11</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Rich Media Specs'!$A$1:$Z$11</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Rich Media Specs'!$A$1:$Z$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Rich Media Specs'!$A$1:$Z$11</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area" vbProcedure="false">'Video Specs'!$A$1:$O$8</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area_0" vbProcedure="false">'Video Specs'!$A$1:$O$8</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Video Specs'!$A$1:$O$8</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Video Specs'!$A$1:$O$8</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Video Specs'!$A$1:$O$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Video Specs'!$A$1:$O$8</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
@@ -188,7 +191,7 @@
     <t>Age 18-34 or Age 34-50 or Education; Columbus Zips</t>
   </si>
   <si>
-    <t>Pre-Roll and 300X250 Companion Ad</t>
+    <t>1x1</t>
   </si>
   <si>
     <t>RON; Columbus Zips</t>
@@ -1401,7 +1404,7 @@
     <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
     <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
     <cellStyle builtinId="8" customBuiltin="false" name="*unknown*" xfId="20"/>
-    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal 2" xfId="21"/>
+    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal 2" xfId="21"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1471,15 +1474,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>239760</xdr:colOff>
+      <xdr:colOff>266760</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>41040</xdr:rowOff>
+      <xdr:rowOff>32040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>471960</xdr:colOff>
+      <xdr:colOff>498600</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>86400</xdr:rowOff>
+      <xdr:rowOff>77040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1494,8 +1497,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="239760" y="183600"/>
-          <a:ext cx="1230120" cy="597960"/>
+          <a:off x="266760" y="174600"/>
+          <a:ext cx="1229760" cy="597600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1510,15 +1513,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>135000</xdr:colOff>
+      <xdr:colOff>162000</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>21600</xdr:rowOff>
+      <xdr:rowOff>12600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>11520</xdr:colOff>
+      <xdr:colOff>38160</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>19800</xdr:rowOff>
+      <xdr:rowOff>10440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1527,8 +1530,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="135000" y="21600"/>
-          <a:ext cx="12354120" cy="45720"/>
+          <a:off x="162000" y="12600"/>
+          <a:ext cx="12353760" cy="45360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1549,15 +1552,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>135000</xdr:colOff>
+      <xdr:colOff>162000</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>155160</xdr:rowOff>
+      <xdr:rowOff>146160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>11520</xdr:colOff>
+      <xdr:colOff>38160</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>38160</xdr:rowOff>
+      <xdr:rowOff>28800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1566,8 +1569,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="135000" y="850320"/>
-          <a:ext cx="12354120" cy="45000"/>
+          <a:off x="162000" y="841320"/>
+          <a:ext cx="12353760" cy="44640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1588,15 +1591,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>135000</xdr:colOff>
+      <xdr:colOff>162000</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>142560</xdr:rowOff>
+      <xdr:rowOff>133560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>49320</xdr:colOff>
+      <xdr:colOff>75960</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>122040</xdr:rowOff>
+      <xdr:rowOff>112680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1605,8 +1608,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="135000" y="4725000"/>
-          <a:ext cx="12391920" cy="141480"/>
+          <a:off x="162000" y="4716000"/>
+          <a:ext cx="12391560" cy="141120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1627,15 +1630,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>135000</xdr:colOff>
+      <xdr:colOff>162000</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>123120</xdr:rowOff>
+      <xdr:rowOff>114120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>39960</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>5760</xdr:rowOff>
+      <xdr:colOff>66600</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>158040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1644,8 +1647,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="135000" y="2936160"/>
-          <a:ext cx="12382560" cy="44280"/>
+          <a:off x="162000" y="2927160"/>
+          <a:ext cx="12382200" cy="43920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1671,15 +1674,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>192240</xdr:colOff>
+      <xdr:colOff>219240</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>12240</xdr:rowOff>
+      <xdr:rowOff>3240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>257040</xdr:colOff>
+      <xdr:colOff>283680</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>210600</xdr:rowOff>
+      <xdr:rowOff>201240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1694,8 +1697,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="192240" y="12240"/>
-          <a:ext cx="1596240" cy="722160"/>
+          <a:off x="219240" y="3240"/>
+          <a:ext cx="1595880" cy="721800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1715,15 +1718,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>239760</xdr:colOff>
+      <xdr:colOff>266760</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>69480</xdr:rowOff>
+      <xdr:rowOff>60480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>304560</xdr:colOff>
+      <xdr:colOff>331200</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>267840</xdr:rowOff>
+      <xdr:rowOff>258480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1738,8 +1741,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="239760" y="69480"/>
-          <a:ext cx="1596240" cy="722160"/>
+          <a:off x="266760" y="60480"/>
+          <a:ext cx="1595880" cy="721800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1759,15 +1762,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>239760</xdr:colOff>
+      <xdr:colOff>266760</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>21600</xdr:rowOff>
+      <xdr:rowOff>12600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>304560</xdr:colOff>
+      <xdr:colOff>331200</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>219960</xdr:rowOff>
+      <xdr:rowOff>210600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1782,8 +1785,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="239760" y="21600"/>
-          <a:ext cx="1596240" cy="722160"/>
+          <a:off x="266760" y="12600"/>
+          <a:ext cx="1595880" cy="721800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1806,7 +1809,7 @@
   <dimension ref="A1:AI172"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="false" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A16" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C30" activeCellId="0" pane="topLeft" sqref="C30"/>
+      <selection activeCell="A31" activeCellId="0" pane="topLeft" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>